<commit_message>
Updating character progress tracker
</commit_message>
<xml_diff>
--- a/talking_heads_ref_files/Character_Progress_Tracker.xlsx
+++ b/talking_heads_ref_files/Character_Progress_Tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Fallout2_Modding\_TALKING_HEADS_MOD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Fallout2_Modding\_TALKING_HEADS_MOD\Fallout2_Talking_Heads\talking_heads_ref_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B60325-602E-4400-BF30-AB86D13396CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145B664C-927C-44E3-BBC2-1CED9F5EC51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{E47AA71F-6854-408C-A1A8-34410F753760}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{E47AA71F-6854-408C-A1A8-34410F753760}"/>
   </bookViews>
   <sheets>
     <sheet name="Status Sheet" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="390">
   <si>
     <t>Klint</t>
   </si>
@@ -366,15 +366,9 @@
     <t>MCCLR</t>
   </si>
   <si>
-    <t>@Wicket</t>
-  </si>
-  <si>
     <t>DAVIN</t>
   </si>
   <si>
-    <t>@ToxicRussian</t>
-  </si>
-  <si>
     <t>Processing</t>
   </si>
   <si>
@@ -390,12 +384,6 @@
     <t>OBAD</t>
   </si>
   <si>
-    <t>Myself</t>
-  </si>
-  <si>
-    <t>@KyoTe44</t>
-  </si>
-  <si>
     <t>@FrozenAmputee</t>
   </si>
   <si>
@@ -408,12 +396,6 @@
     <t>@optical</t>
   </si>
   <si>
-    <t>georgejparker08@gmail.com</t>
-  </si>
-  <si>
-    <t>symesad@gmail.com</t>
-  </si>
-  <si>
     <t>Jules</t>
   </si>
   <si>
@@ -438,15 +420,9 @@
     <t>BIRD</t>
   </si>
   <si>
-    <t>khristonrobinson@gmail.com</t>
-  </si>
-  <si>
     <t>JOMOD</t>
   </si>
   <si>
-    <t>@SoldierPaladin</t>
-  </si>
-  <si>
     <t>DAN</t>
   </si>
   <si>
@@ -465,15 +441,9 @@
     <t>BADGE</t>
   </si>
   <si>
-    <t>@TheOtherGrom</t>
-  </si>
-  <si>
     <t>Vikki &amp; Juan</t>
   </si>
   <si>
-    <t>jenna.de.j2@gmail.com</t>
-  </si>
-  <si>
     <t>SCH</t>
   </si>
   <si>
@@ -516,9 +486,6 @@
     <t>SKY</t>
   </si>
   <si>
-    <t>joannereadxxx@gmail.com</t>
-  </si>
-  <si>
     <t>ELISE</t>
   </si>
   <si>
@@ -630,9 +597,6 @@
     <t>VAJ</t>
   </si>
   <si>
-    <t>@brasch747</t>
-  </si>
-  <si>
     <t>brannonbraxton4@gmail.com</t>
   </si>
   <si>
@@ -642,12 +606,6 @@
     <t>DRAGO</t>
   </si>
   <si>
-    <t>@d.flowerrs</t>
-  </si>
-  <si>
-    <t>@DoraTrix</t>
-  </si>
-  <si>
     <t>Steve</t>
   </si>
   <si>
@@ -882,9 +840,6 @@
     <t>Ella Gans / Coolartist1110</t>
   </si>
   <si>
-    <t>NoisyRooster#6891</t>
-  </si>
-  <si>
     <t xml:space="preserve">@GlyphDawn </t>
   </si>
   <si>
@@ -894,9 +849,6 @@
     <t>@Balmus</t>
   </si>
   <si>
-    <t>@izzfizz14</t>
-  </si>
-  <si>
     <t>shiisaicecream@proton.me</t>
   </si>
   <si>
@@ -1080,9 +1032,6 @@
     <t>Donkey</t>
   </si>
   <si>
-    <t>@AlexDewhurstVA</t>
-  </si>
-  <si>
     <t>Check Email</t>
   </si>
   <si>
@@ -1107,9 +1056,6 @@
     <t>Morgan Fox / @Flamekebab</t>
   </si>
   <si>
-    <t>gonsqua for AHS-7 | Casting Call Club</t>
-  </si>
-  <si>
     <t>Dubbed One for Mayor Ascorti | Casting Call Club</t>
   </si>
   <si>
@@ -1125,9 +1071,6 @@
     <t>https://www.castingcall.club/auditions/2704390</t>
   </si>
   <si>
-    <t>https://www.castingcall.club/auditions/2704382</t>
-  </si>
-  <si>
     <t>ClaireM</t>
   </si>
   <si>
@@ -1143,9 +1086,6 @@
     <t>@Mop</t>
   </si>
   <si>
-    <t>@SpaceIshmael</t>
-  </si>
-  <si>
     <t>@D E A D</t>
   </si>
   <si>
@@ -1234,12 +1174,6 @@
   </si>
   <si>
     <t>@Jerkytown</t>
-  </si>
-  <si>
-    <t>@Dwig</t>
-  </si>
-  <si>
-    <t>dillon820g@gmail.com</t>
   </si>
   <si>
     <t>@Banana Pancakes</t>
@@ -1945,10 +1879,10 @@
   <dimension ref="A1:AM148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J42" sqref="J42"/>
+      <selection pane="bottomRight" activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1984,7 +1918,7 @@
         <v>99</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
@@ -2000,16 +1934,16 @@
         <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="1"/>
@@ -2048,16 +1982,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="1"/>
@@ -2093,21 +2027,19 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>355</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="F4" s="14"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2141,20 +2073,20 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -2192,16 +2124,16 @@
         <v>57</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="1"/>
@@ -2237,7 +2169,7 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>98</v>
@@ -2247,7 +2179,7 @@
         <v>36</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="1"/>
@@ -2283,17 +2215,17 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="1"/>
@@ -2339,7 +2271,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="1"/>
@@ -2378,18 +2310,16 @@
         <v>81</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>134</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F10" s="14"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -2423,22 +2353,22 @@
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>404</v>
+        <v>382</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -2473,19 +2403,19 @@
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="1"/>
@@ -2521,20 +2451,20 @@
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -2572,7 +2502,7 @@
         <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
@@ -2581,9 +2511,7 @@
       <c r="E14" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>399</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2617,7 +2545,7 @@
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>95</v>
@@ -2627,7 +2555,7 @@
         <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
@@ -2663,7 +2591,7 @@
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>95</v>
@@ -2673,7 +2601,7 @@
         <v>37</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
@@ -2709,19 +2637,19 @@
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
@@ -2757,20 +2685,20 @@
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="1"/>
@@ -2808,17 +2736,17 @@
         <v>75</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
         <v>78</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2853,17 +2781,17 @@
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
@@ -2902,10 +2830,10 @@
         <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>35</v>
@@ -2950,18 +2878,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>118</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="F22" s="3"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2995,7 +2921,7 @@
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>95</v>
@@ -3005,7 +2931,7 @@
         <v>87</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="1"/>
@@ -3041,7 +2967,7 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>95</v>
@@ -3051,7 +2977,7 @@
         <v>90</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="1"/>
@@ -3090,18 +3016,16 @@
         <v>74</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>72</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>122</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="F25" s="14"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -3135,7 +3059,7 @@
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>95</v>
@@ -3145,7 +3069,7 @@
         <v>62</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="1"/>
@@ -3184,18 +3108,16 @@
         <v>3</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>196</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="F27" s="3"/>
       <c r="G27" s="4"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -3229,7 +3151,7 @@
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>95</v>
@@ -3239,7 +3161,7 @@
         <v>28</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="1"/>
@@ -3275,22 +3197,22 @@
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A29" s="26" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="1"/>
@@ -3331,7 +3253,7 @@
         <v>72</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="4"/>
@@ -3370,17 +3292,17 @@
         <v>42</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="1"/>
@@ -3425,7 +3347,7 @@
         <v>72</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="1"/>
@@ -3461,7 +3383,7 @@
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>95</v>
@@ -3471,7 +3393,7 @@
         <v>37</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="1"/>
@@ -3510,18 +3432,16 @@
         <v>25</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F34" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="F34" s="3"/>
       <c r="G34" s="4"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -3558,16 +3478,16 @@
         <v>77</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>78</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="4"/>
@@ -3606,7 +3526,7 @@
         <v>41</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
@@ -3651,18 +3571,16 @@
         <v>8</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>116</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="F37" s="3"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -3696,17 +3614,17 @@
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="1"/>
@@ -3742,17 +3660,17 @@
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="3" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="1"/>
@@ -3791,16 +3709,16 @@
         <v>65</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>68</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="1"/>
@@ -3839,16 +3757,16 @@
         <v>89</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>401</v>
+        <v>379</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>90</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F41" s="14"/>
       <c r="G41" s="1"/>
@@ -3887,19 +3805,19 @@
         <v>31</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="12"/>
@@ -3944,7 +3862,7 @@
         <v>87</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="1"/>
@@ -3980,19 +3898,19 @@
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="1"/>
@@ -4031,18 +3949,16 @@
         <v>67</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
         <v>68</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>158</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="F45" s="3"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -4076,7 +3992,7 @@
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>95</v>
@@ -4086,7 +4002,7 @@
         <v>68</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="1"/>
@@ -4122,7 +4038,7 @@
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>95</v>
@@ -4132,7 +4048,7 @@
         <v>62</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="1"/>
@@ -4178,7 +4094,7 @@
         <v>46</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="1"/>
@@ -4214,7 +4130,7 @@
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>95</v>
@@ -4224,7 +4140,7 @@
         <v>28</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="1"/>
@@ -4263,17 +4179,17 @@
         <v>60</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -4308,22 +4224,22 @@
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -4361,18 +4277,16 @@
         <v>47</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>123</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="F52" s="14"/>
       <c r="G52" s="4"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -4406,20 +4320,20 @@
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="1"/>
@@ -4454,22 +4368,22 @@
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="1"/>
@@ -4507,7 +4421,7 @@
         <v>69</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
@@ -4516,9 +4430,7 @@
       <c r="E55" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="F55" s="3"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -4552,17 +4464,17 @@
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="1"/>
@@ -4598,7 +4510,7 @@
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>95</v>
@@ -4608,7 +4520,7 @@
         <v>28</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="1"/>
@@ -4647,18 +4559,16 @@
         <v>70</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F58" s="19" t="s">
-        <v>280</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="F58" s="19"/>
       <c r="G58" s="4"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -4692,7 +4602,7 @@
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>95</v>
@@ -4702,7 +4612,7 @@
         <v>35</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="F59" s="19"/>
       <c r="G59" s="4"/>
@@ -4738,20 +4648,20 @@
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>408</v>
+        <v>386</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -4796,7 +4706,7 @@
         <v>12</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="1"/>
@@ -4832,7 +4742,7 @@
     </row>
     <row r="62" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>95</v>
@@ -4842,7 +4752,7 @@
         <v>62</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="1"/>
@@ -4881,18 +4791,16 @@
         <v>27</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F63" s="14" t="s">
-        <v>132</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="F63" s="14"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -4929,16 +4837,16 @@
         <v>18</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="4"/>
@@ -4974,17 +4882,17 @@
     </row>
     <row r="65" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="F65" s="3"/>
       <c r="G65" s="1"/>
@@ -5020,21 +4928,19 @@
     </row>
     <row r="66" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>110</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F66" s="3"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -5071,19 +4977,19 @@
         <v>88</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>90</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="1"/>
@@ -5118,7 +5024,7 @@
     </row>
     <row r="68" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>95</v>
@@ -5128,7 +5034,7 @@
         <v>11</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="1"/>
@@ -5164,7 +5070,7 @@
     </row>
     <row r="69" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>95</v>
@@ -5174,7 +5080,7 @@
         <v>62</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="4"/>
@@ -5213,16 +5119,16 @@
         <v>79</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="F70" s="14"/>
       <c r="G70" s="1"/>
@@ -5261,18 +5167,16 @@
         <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
         <v>78</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>284</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="F71" s="3"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
@@ -5309,10 +5213,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>11</v>
@@ -5354,7 +5258,7 @@
     </row>
     <row r="73" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>95</v>
@@ -5364,7 +5268,7 @@
         <v>23</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="1"/>
@@ -5400,7 +5304,7 @@
     </row>
     <row r="74" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>95</v>
@@ -5410,7 +5314,7 @@
         <v>23</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="F74" s="3"/>
       <c r="G74" s="1"/>
@@ -5446,7 +5350,7 @@
     </row>
     <row r="75" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>95</v>
@@ -5456,7 +5360,7 @@
         <v>28</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="1"/>
@@ -5495,16 +5399,16 @@
         <v>84</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="F76" s="3"/>
       <c r="G76" s="1"/>
@@ -5543,17 +5447,17 @@
         <v>22</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F77" t="s">
-        <v>409</v>
+        <v>387</v>
       </c>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
@@ -5591,7 +5495,7 @@
         <v>4</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>344</v>
+        <v>96</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
@@ -5601,7 +5505,7 @@
         <v>102</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" s="4"/>
@@ -5646,7 +5550,7 @@
         <v>62</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="1"/>
@@ -5685,16 +5589,16 @@
         <v>51</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F80" s="3"/>
       <c r="G80" s="1"/>
@@ -5740,7 +5644,7 @@
         <v>87</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="1"/>
@@ -5776,21 +5680,19 @@
     </row>
     <row r="82" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>201</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="F82" s="3"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
@@ -5824,7 +5726,7 @@
     </row>
     <row r="83" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>95</v>
@@ -5834,7 +5736,7 @@
         <v>35</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="1"/>
@@ -5880,7 +5782,7 @@
         <v>12</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="1"/>
@@ -5926,7 +5828,7 @@
         <v>46</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="1"/>
@@ -5965,18 +5867,16 @@
         <v>61</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>201</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F86" s="3"/>
       <c r="G86" s="4"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
@@ -6013,18 +5913,16 @@
         <v>53</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>200</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="F87" s="3"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
@@ -6061,19 +5959,19 @@
         <v>86</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>402</v>
+        <v>380</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
@@ -6118,10 +6016,10 @@
         <v>46</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
@@ -6156,21 +6054,19 @@
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
         <v>68</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>346</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="F90" s="3"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -6207,18 +6103,16 @@
         <v>19</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>196</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="F91" s="3"/>
       <c r="G91" s="4"/>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
@@ -6255,16 +6149,16 @@
         <v>63</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>68</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F92" s="14"/>
       <c r="G92" s="4"/>
@@ -6303,17 +6197,17 @@
         <v>24</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="F93" s="21" t="s">
-        <v>410</v>
+        <v>388</v>
       </c>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
@@ -6351,16 +6245,16 @@
         <v>20</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F94" s="3"/>
       <c r="G94" s="1"/>
@@ -6399,14 +6293,14 @@
         <v>55</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="1"/>
@@ -6445,17 +6339,17 @@
         <v>58</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
@@ -6490,20 +6384,20 @@
     </row>
     <row r="97" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
@@ -6538,7 +6432,7 @@
     </row>
     <row r="98" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>95</v>
@@ -6548,7 +6442,7 @@
         <v>90</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="F98" s="3"/>
       <c r="G98" s="1"/>
@@ -6584,19 +6478,19 @@
     </row>
     <row r="99" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="F99" s="3"/>
       <c r="G99" s="1"/>
@@ -6635,16 +6529,16 @@
         <v>44</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F100" s="18"/>
       <c r="G100" s="1"/>
@@ -6679,7 +6573,7 @@
     </row>
     <row r="101" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>95</v>
@@ -6689,7 +6583,7 @@
         <v>35</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="F101" s="18"/>
       <c r="G101" s="1"/>
@@ -6727,18 +6621,16 @@
         <v>54</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F102" s="14" t="s">
-        <v>120</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="F102" s="14"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
@@ -6772,7 +6664,7 @@
     </row>
     <row r="103" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>95</v>
@@ -6782,7 +6674,7 @@
         <v>37</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
       <c r="F103" s="14"/>
       <c r="G103" s="1"/>
@@ -6821,18 +6713,16 @@
         <v>32</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F104" s="14" t="s">
-        <v>143</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="F104" s="14"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
@@ -6866,22 +6756,22 @@
     </row>
     <row r="105" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="F105" s="14" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
@@ -6916,7 +6806,7 @@
     </row>
     <row r="106" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A106" s="15" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B106" s="15" t="s">
         <v>95</v>
@@ -6926,7 +6816,7 @@
         <v>90</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="F106" s="3"/>
       <c r="G106" s="1"/>
@@ -6962,7 +6852,7 @@
     </row>
     <row r="107" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A107" s="15" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="B107" s="15" t="s">
         <v>95</v>
@@ -6970,7 +6860,7 @@
       <c r="C107" s="23"/>
       <c r="D107" s="25"/>
       <c r="E107" s="3" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="F107" s="3"/>
       <c r="G107" s="1"/>
@@ -7006,7 +6896,7 @@
     </row>
     <row r="108" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A108" s="16" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>95</v>
@@ -7016,7 +6906,7 @@
         <v>90</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="F108" s="3"/>
       <c r="G108" s="1"/>
@@ -7052,7 +6942,7 @@
     </row>
     <row r="109" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A109" s="16" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="B109" s="15" t="s">
         <v>95</v>
@@ -7062,7 +6952,7 @@
         <v>90</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="F109" s="3"/>
       <c r="G109" s="1"/>
@@ -7098,7 +6988,7 @@
     </row>
     <row r="110" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>95</v>
@@ -7108,7 +6998,7 @@
         <v>72</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="F110" s="3"/>
       <c r="G110" s="1"/>
@@ -7144,20 +7034,20 @@
     </row>
     <row r="111" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="F111" s="14" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
@@ -7192,20 +7082,20 @@
     </row>
     <row r="112" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
@@ -7250,7 +7140,7 @@
         <v>68</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="F113" s="14"/>
       <c r="G113" s="1"/>
@@ -7289,7 +7179,7 @@
         <v>64</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3" t="s">
@@ -7299,7 +7189,7 @@
         <v>106</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G114" s="4"/>
       <c r="H114" s="1"/>
@@ -7344,7 +7234,7 @@
         <v>28</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F115" s="3"/>
       <c r="G115" s="1"/>
@@ -7380,7 +7270,7 @@
     </row>
     <row r="116" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>95</v>
@@ -7390,7 +7280,7 @@
         <v>12</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="F116" s="3"/>
       <c r="G116" s="1"/>
@@ -7429,17 +7319,17 @@
         <v>52</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>401</v>
+        <v>379</v>
       </c>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
@@ -7474,17 +7364,17 @@
     </row>
     <row r="118" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="F118" s="14"/>
       <c r="G118" s="1"/>
@@ -7520,20 +7410,20 @@
     </row>
     <row r="119" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C119" s="7"/>
       <c r="D119" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
@@ -7568,17 +7458,17 @@
     </row>
     <row r="120" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="F120" s="14"/>
       <c r="G120" s="1"/>
@@ -7614,7 +7504,7 @@
     </row>
     <row r="121" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>95</v>
@@ -7624,7 +7514,7 @@
         <v>68</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="1"/>
@@ -7663,7 +7553,7 @@
         <v>39</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3" t="s">
@@ -7673,7 +7563,7 @@
         <v>105</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G122" s="4"/>
       <c r="H122" s="1"/>
@@ -7708,21 +7598,19 @@
     </row>
     <row r="123" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F123" s="3" t="s">
-        <v>367</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="F123" s="3"/>
       <c r="G123" s="4"/>
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
@@ -7759,17 +7647,17 @@
         <v>6</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="G124" s="1"/>
       <c r="H124" s="4"/>
@@ -7804,19 +7692,19 @@
     </row>
     <row r="125" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="F125" s="14"/>
       <c r="G125" s="4"/>
@@ -7855,16 +7743,16 @@
         <v>15</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F126" s="3"/>
       <c r="G126" s="4"/>
@@ -7900,22 +7788,22 @@
     </row>
     <row r="127" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
@@ -7953,19 +7841,19 @@
         <v>33</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F128" s="18" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="G128" s="12"/>
       <c r="H128" s="1"/>
@@ -8000,22 +7888,22 @@
     </row>
     <row r="129" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="G129" s="4"/>
       <c r="H129" s="1"/>
@@ -8053,17 +7941,17 @@
         <v>59</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C130" s="3"/>
       <c r="D130" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="F130" s="14" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
@@ -8108,7 +7996,7 @@
         <v>87</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="F131" s="3"/>
       <c r="G131" s="1"/>
@@ -8144,22 +8032,22 @@
     </row>
     <row r="132" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
@@ -8194,7 +8082,7 @@
     </row>
     <row r="133" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>95</v>
@@ -8204,7 +8092,7 @@
         <v>35</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="F133" s="3"/>
       <c r="G133" s="1"/>
@@ -8240,21 +8128,19 @@
     </row>
     <row r="134" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C134" s="3"/>
       <c r="D134" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="F134" s="14" t="s">
-        <v>361</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="F134" s="14"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
@@ -8291,16 +8177,16 @@
         <v>17</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F135" s="3"/>
       <c r="G135" s="1"/>
@@ -8339,16 +8225,16 @@
         <v>48</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F136" s="3"/>
       <c r="G136" s="1"/>
@@ -8387,17 +8273,17 @@
         <v>34</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C137" s="3"/>
       <c r="D137" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>405</v>
+        <v>383</v>
       </c>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
@@ -8442,7 +8328,7 @@
         <v>29</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F138" s="3"/>
       <c r="G138" s="1"/>
@@ -8480,18 +8366,16 @@
         <v>21</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C139" s="3"/>
       <c r="D139" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F139" s="20" t="s">
-        <v>398</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="F139" s="20"/>
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
       <c r="I139" s="4"/>
@@ -8528,18 +8412,16 @@
         <v>7</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F140" s="3" t="s">
-        <v>141</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="F140" s="3"/>
       <c r="G140" s="4"/>
       <c r="H140" s="1"/>
       <c r="I140" s="1"/>
@@ -8573,21 +8455,19 @@
     </row>
     <row r="141" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F141" s="3" t="s">
-        <v>201</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="F141" s="3"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
@@ -8621,7 +8501,7 @@
     </row>
     <row r="142" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>95</v>
@@ -8631,7 +8511,7 @@
         <v>68</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="F142" s="3"/>
       <c r="G142" s="1"/>
@@ -8667,20 +8547,20 @@
     </row>
     <row r="143" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="F143" s="14" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
@@ -8715,19 +8595,19 @@
     </row>
     <row r="144" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F144" s="14"/>
       <c r="G144" s="1"/>
@@ -8763,16 +8643,16 @@
     </row>
     <row r="145" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>90</v>
       </c>
       <c r="E145" s="13" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="F145" s="14"/>
       <c r="G145" s="1"/>
@@ -8808,7 +8688,7 @@
     </row>
     <row r="146" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>95</v>
@@ -8818,7 +8698,7 @@
         <v>49</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="F146" s="3"/>
       <c r="G146" s="1"/>
@@ -8854,7 +8734,7 @@
     </row>
     <row r="147" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>95</v>
@@ -8864,7 +8744,7 @@
         <v>72</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="F147" s="3"/>
       <c r="G147" s="1"/>
@@ -8900,7 +8780,7 @@
     </row>
     <row r="148" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>95</v>
@@ -8910,7 +8790,7 @@
         <v>38</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="F148" s="3"/>
       <c r="G148" s="1"/>
@@ -8963,22 +8843,14 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F114" r:id="rId1" xr:uid="{C98809CD-4E10-4A14-A2B8-4F831C04652C}"/>
-    <hyperlink ref="F25" r:id="rId2" xr:uid="{A9A813D1-7185-4D1E-8868-765FB305A5ED}"/>
-    <hyperlink ref="F63" r:id="rId3" xr:uid="{7CD30038-E330-4D14-B53E-795E518D3A96}"/>
-    <hyperlink ref="F52" r:id="rId4" xr:uid="{561AA50A-388B-453A-A0AD-6B580D87B562}"/>
-    <hyperlink ref="F102" r:id="rId5" xr:uid="{48E32B94-5B86-4906-95C5-46EA3E438B09}"/>
-    <hyperlink ref="F10" r:id="rId6" display="keith.edward.dwyer@gmail.com" xr:uid="{C9BF2E44-7E27-4C21-9982-BC051291B73F}"/>
-    <hyperlink ref="F104" r:id="rId7" display="http://jenna.de/" xr:uid="{D03D4B34-63FC-42A3-AE38-58B3FAC83123}"/>
-    <hyperlink ref="F31" r:id="rId8" xr:uid="{6A4861FA-3BAA-43F0-B05A-C4DC611C6CDF}"/>
-    <hyperlink ref="F4" r:id="rId9" display="https://www.castingcall.club/submissions/2855371" xr:uid="{C64D57F4-4A7D-40B7-A436-94B282FA4496}"/>
-    <hyperlink ref="F89" r:id="rId10" display="https://www.castingcall.club/submissions/2749165" xr:uid="{8FBA86C6-D92F-43C1-B6A2-B545AEBC0F06}"/>
-    <hyperlink ref="F96" r:id="rId11" display="https://www.castingcall.club/submissions/2747679" xr:uid="{EE4B43D0-534D-41C4-98DC-B3E87558E155}"/>
-    <hyperlink ref="F111" r:id="rId12" display="https://www.castingcall.club/submissions/2747649" xr:uid="{758647D1-B48D-43E4-9060-01C3C48582D6}"/>
-    <hyperlink ref="F53" r:id="rId13" tooltip="https://www.castingcall.club/auditions/2704390" xr:uid="{E67C3744-7F6A-4CBB-9D31-5E01F52825A0}"/>
-    <hyperlink ref="F134" r:id="rId14" tooltip="https://www.castingcall.club/auditions/2704382" xr:uid="{D4DC5275-75A1-4F56-BBED-8569CF742DE1}"/>
+    <hyperlink ref="F31" r:id="rId2" xr:uid="{6A4861FA-3BAA-43F0-B05A-C4DC611C6CDF}"/>
+    <hyperlink ref="F89" r:id="rId3" display="https://www.castingcall.club/submissions/2749165" xr:uid="{8FBA86C6-D92F-43C1-B6A2-B545AEBC0F06}"/>
+    <hyperlink ref="F96" r:id="rId4" display="https://www.castingcall.club/submissions/2747679" xr:uid="{EE4B43D0-534D-41C4-98DC-B3E87558E155}"/>
+    <hyperlink ref="F111" r:id="rId5" display="https://www.castingcall.club/submissions/2747649" xr:uid="{758647D1-B48D-43E4-9060-01C3C48582D6}"/>
+    <hyperlink ref="F53" r:id="rId6" tooltip="https://www.castingcall.club/auditions/2704390" xr:uid="{E67C3744-7F6A-4CBB-9D31-5E01F52825A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -9160,10 +9032,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -9184,7 +9056,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>49</v>
@@ -9195,12 +9067,12 @@
         <v>96</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>91</v>
@@ -9216,7 +9088,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>38</v>
@@ -9224,7 +9096,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>29</v>
@@ -9232,7 +9104,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>12</v>
@@ -9240,7 +9112,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>28</v>
@@ -9248,7 +9120,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>90</v>
@@ -9256,7 +9128,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>68</v>
@@ -9264,7 +9136,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>62</v>
@@ -9272,7 +9144,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" s="11" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -9292,7 +9164,7 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="11" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>